<commit_message>
Added Json file implementations
</commit_message>
<xml_diff>
--- a/test_data/Website_login.xlsx
+++ b/test_data/Website_login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hybrid_framework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110B5313-C821-4952-9D49-3553CDE02342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF15279-3FAA-4754-B001-665850F459ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{89B7A792-C47B-4B6E-A0AC-00AD5C6E4DD9}"/>
   </bookViews>
@@ -62,7 +62,7 @@
     <t>C:\Users\148592\OneDrive - Arrow Electronics, Inc\Desktop\python\Python.txt</t>
   </si>
   <si>
-    <t>C:\Users\148592\OneDrive - Arrow Electronics, Inc\Desktop\Proof\Books_proof</t>
+    <t>C:\Users\148592\OneDrive - Arrow Electronics, Inc\Desktop\Proof\Books_proof.pdf</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>